<commit_message>
Replace USGS NWIS data with updated dataset through June 2025 from new USGS WDFN website
Also removed fields specific to NWIS from all other datasets
</commit_message>
<xml_diff>
--- a/data-raw/formatted_data/USGS_Tributary_Study.xlsx
+++ b/data-raw/formatted_data/USGS_Tributary_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ltimaofile01.limno.com\Projects\DDOEIP\Water Quality Program Update\Impairment Assessment Updates\ImpairmentReview_2020\Analysis_Fall_2022\formatted_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srucker\Git\IRsupportR\data-raw\formatted_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B435B686-F6C2-4D30-A2FD-D03F47E64E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F3EA8D-3B50-4290-9DB6-A04D20B46E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A06C9829-9A1D-49BA-A504-3D5E251AF0A7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A06C9829-9A1D-49BA-A504-3D5E251AF0A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Formatted" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3471" uniqueCount="114">
   <si>
     <t>ALUMINUM (7429-90-5)</t>
   </si>
@@ -373,21 +373,6 @@
     <t>reporting_level_type</t>
   </si>
   <si>
-    <t>time_datum_code</t>
-  </si>
-  <si>
-    <t>time_datum_reliability_code</t>
-  </si>
-  <si>
-    <t>parameter_code</t>
-  </si>
-  <si>
-    <t>qualifier_code</t>
-  </si>
-  <si>
-    <t>data_quality_code</t>
-  </si>
-  <si>
     <t>result_notes</t>
   </si>
   <si>
@@ -452,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -492,7 +477,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -598,7 +583,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -740,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -748,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBCA466-84A1-4AA9-9D9B-6106C03A76B4}">
-  <dimension ref="A1:AB323"/>
+  <dimension ref="A1:W323"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -779,14 +764,9 @@
     <col min="21" max="21" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20" customWidth="1"/>
-    <col min="24" max="24" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -830,7 +810,7 @@
         <v>28</v>
       </c>
       <c r="O1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="P1" t="s">
         <v>105</v>
@@ -845,7 +825,7 @@
         <v>107</v>
       </c>
       <c r="T1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="U1" t="s">
         <v>109</v>
@@ -854,25 +834,10 @@
         <v>110</v>
       </c>
       <c r="W1" t="s">
-        <v>118</v>
-      </c>
-      <c r="X1" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z1" t="s">
         <v>113</v>
       </c>
-      <c r="AA1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -910,7 +875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -951,7 +916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -989,7 +954,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -1027,7 +992,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -1068,7 +1033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -1109,7 +1074,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -1147,7 +1112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -1185,7 +1150,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -1223,7 +1188,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -1264,7 +1229,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -1302,7 +1267,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -1340,7 +1305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -1378,7 +1343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -1416,7 +1381,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>108</v>
       </c>

</xml_diff>